<commit_message>
docs: Creating Department api file
</commit_message>
<xml_diff>
--- a/api/Notice/Department_API.xlsx
+++ b/api/Notice/Department_API.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Notice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A1C2FE-8E04-4FD6-B302-AEFE4BCE86A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01793DF-21F2-47AA-8AB1-8F63BADCCD74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="학과 공지 전체 조회" sheetId="1" r:id="rId1"/>
-    <sheet name="학교 공지 상세 조회" sheetId="2" r:id="rId2"/>
-    <sheet name="학교 공지 작성" sheetId="3" r:id="rId3"/>
-    <sheet name="학교 공지 수정" sheetId="4" r:id="rId4"/>
-    <sheet name="학교 공지 삭제" sheetId="5" r:id="rId5"/>
+    <sheet name="학과 공지 상세 조회" sheetId="2" r:id="rId2"/>
+    <sheet name="학과 공지 작성" sheetId="3" r:id="rId3"/>
+    <sheet name="학과 공지 수정" sheetId="4" r:id="rId4"/>
+    <sheet name="학과 공지 삭제" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1535,17 +1535,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1557,20 +1561,16 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1600,6 +1600,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1608,15 +1623,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1634,12 +1640,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1973,95 +1973,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -2110,64 +2110,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="38"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -2502,28 +2502,28 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" ht="343" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" ht="349.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -3098,6 +3098,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
@@ -3106,12 +3112,6 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3142,29 +3142,29 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -3184,53 +3184,53 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -3289,64 +3289,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="38"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -3681,28 +3681,28 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" ht="255.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" ht="269.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -4277,6 +4277,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
@@ -4285,12 +4291,6 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4321,29 +4321,29 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -4363,53 +4363,53 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -4748,28 +4748,28 @@
       <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:8" ht="198.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="54"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
@@ -5118,28 +5118,28 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="33"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" ht="257" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
     </row>
     <row r="49" spans="1:8" ht="271" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
@@ -5464,12 +5464,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A46:H46"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -5477,6 +5471,12 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -5507,29 +5507,29 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -5549,53 +5549,53 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -5934,42 +5934,42 @@
       <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:13" ht="260" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="54"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="51"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="56"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="21" t="s">
@@ -6048,11 +6048,11 @@
         <v>32</v>
       </c>
       <c r="H32" s="22"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="22" t="s">
@@ -6309,28 +6309,28 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="33"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" ht="267.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
     </row>
     <row r="49" spans="1:8" ht="277" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="50" spans="1:8" ht="271" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6656,11 +6656,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="A46:H46"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -6668,6 +6663,11 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="A46:H46"/>
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A27:H27"/>
@@ -6686,7 +6686,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -6701,29 +6701,29 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -6743,53 +6743,53 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -6862,40 +6862,40 @@
       <c r="H11" s="48"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="59"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
@@ -6978,28 +6978,28 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
     </row>
     <row r="20" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="13"/>
@@ -7122,24 +7122,24 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="55"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="56"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
@@ -7743,13 +7743,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
@@ -7759,6 +7752,13 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>